<commit_message>
começando a fazer as equações de area relativa da 7.6
</commit_message>
<xml_diff>
--- a/doc/ACAP DG PH 7.6 31-03-21.xlsx
+++ b/doc/ACAP DG PH 7.6 31-03-21.xlsx
@@ -1124,11 +1124,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="101894400"/>
-        <c:axId val="101900288"/>
+        <c:axId val="95279744"/>
+        <c:axId val="95281536"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="101894400"/>
+        <c:axId val="95279744"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1137,7 +1137,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="101900288"/>
+        <c:crossAx val="95281536"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1145,7 +1145,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="101900288"/>
+        <c:axId val="95281536"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1156,7 +1156,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="101894400"/>
+        <c:crossAx val="95279744"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1369,11 +1369,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="106784256"/>
-        <c:axId val="106785792"/>
+        <c:axId val="105150336"/>
+        <c:axId val="105151872"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="106784256"/>
+        <c:axId val="105150336"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1382,7 +1382,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="106785792"/>
+        <c:crossAx val="105151872"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1390,7 +1390,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="106785792"/>
+        <c:axId val="105151872"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1401,7 +1401,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="106784256"/>
+        <c:crossAx val="105150336"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1614,11 +1614,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="106813312"/>
-        <c:axId val="106814848"/>
+        <c:axId val="105175296"/>
+        <c:axId val="105193472"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="106813312"/>
+        <c:axId val="105175296"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1627,7 +1627,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="106814848"/>
+        <c:crossAx val="105193472"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1635,7 +1635,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="106814848"/>
+        <c:axId val="105193472"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1646,7 +1646,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="106813312"/>
+        <c:crossAx val="105175296"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1859,11 +1859,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="106457344"/>
-        <c:axId val="106467328"/>
+        <c:axId val="105212544"/>
+        <c:axId val="105222528"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="106457344"/>
+        <c:axId val="105212544"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1872,7 +1872,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="106467328"/>
+        <c:crossAx val="105222528"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1880,7 +1880,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="106467328"/>
+        <c:axId val="105222528"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1891,7 +1891,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="106457344"/>
+        <c:crossAx val="105212544"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2104,11 +2104,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="106564224"/>
-        <c:axId val="106574208"/>
+        <c:axId val="105389056"/>
+        <c:axId val="105399040"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="106564224"/>
+        <c:axId val="105389056"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2117,7 +2117,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="106574208"/>
+        <c:crossAx val="105399040"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2125,7 +2125,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="106574208"/>
+        <c:axId val="105399040"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2136,7 +2136,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="106564224"/>
+        <c:crossAx val="105389056"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2349,11 +2349,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="106601472"/>
-        <c:axId val="106619648"/>
+        <c:axId val="105426304"/>
+        <c:axId val="105440384"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="106601472"/>
+        <c:axId val="105426304"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2362,7 +2362,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="106619648"/>
+        <c:crossAx val="105440384"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2370,7 +2370,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="106619648"/>
+        <c:axId val="105440384"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2381,7 +2381,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="106601472"/>
+        <c:crossAx val="105426304"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2594,11 +2594,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="106646912"/>
-        <c:axId val="106665088"/>
+        <c:axId val="105484288"/>
+        <c:axId val="105485824"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="106646912"/>
+        <c:axId val="105484288"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2607,7 +2607,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="106665088"/>
+        <c:crossAx val="105485824"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2615,7 +2615,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="106665088"/>
+        <c:axId val="105485824"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2626,7 +2626,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="106646912"/>
+        <c:crossAx val="105484288"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2839,11 +2839,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="102050432"/>
-        <c:axId val="102060416"/>
+        <c:axId val="96750592"/>
+        <c:axId val="96760576"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="102050432"/>
+        <c:axId val="96750592"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2852,7 +2852,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="102060416"/>
+        <c:crossAx val="96760576"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2860,7 +2860,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="102060416"/>
+        <c:axId val="96760576"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2871,7 +2871,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="102050432"/>
+        <c:crossAx val="96750592"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3089,11 +3089,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="106368000"/>
-        <c:axId val="106373888"/>
+        <c:axId val="102305152"/>
+        <c:axId val="102311040"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="106368000"/>
+        <c:axId val="102305152"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3102,7 +3102,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="106373888"/>
+        <c:crossAx val="102311040"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3110,7 +3110,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="106373888"/>
+        <c:axId val="102311040"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3121,7 +3121,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="106368000"/>
+        <c:crossAx val="102305152"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3334,11 +3334,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="106398848"/>
-        <c:axId val="106400384"/>
+        <c:axId val="102350848"/>
+        <c:axId val="102352384"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="106398848"/>
+        <c:axId val="102350848"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3347,7 +3347,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="106400384"/>
+        <c:crossAx val="102352384"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3355,7 +3355,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="106400384"/>
+        <c:axId val="102352384"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3366,7 +3366,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="106398848"/>
+        <c:crossAx val="102350848"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3579,11 +3579,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="106125184"/>
-        <c:axId val="106126720"/>
+        <c:axId val="105271680"/>
+        <c:axId val="105273216"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="106125184"/>
+        <c:axId val="105271680"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3592,7 +3592,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="106126720"/>
+        <c:crossAx val="105273216"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3600,7 +3600,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="106126720"/>
+        <c:axId val="105273216"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3611,7 +3611,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="106125184"/>
+        <c:crossAx val="105271680"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3824,11 +3824,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="106154240"/>
-        <c:axId val="106237952"/>
+        <c:axId val="104928384"/>
+        <c:axId val="104929920"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="106154240"/>
+        <c:axId val="104928384"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3837,7 +3837,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="106237952"/>
+        <c:crossAx val="104929920"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3845,7 +3845,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="106237952"/>
+        <c:axId val="104929920"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3856,7 +3856,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="106154240"/>
+        <c:crossAx val="104928384"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4069,11 +4069,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="106267392"/>
-        <c:axId val="106268928"/>
+        <c:axId val="104960768"/>
+        <c:axId val="104962304"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="106267392"/>
+        <c:axId val="104960768"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4082,7 +4082,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="106268928"/>
+        <c:crossAx val="104962304"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4090,7 +4090,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="106268928"/>
+        <c:axId val="104962304"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4101,7 +4101,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="106267392"/>
+        <c:crossAx val="104960768"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4314,11 +4314,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="106304256"/>
-        <c:axId val="106305792"/>
+        <c:axId val="105075840"/>
+        <c:axId val="105077376"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="106304256"/>
+        <c:axId val="105075840"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4327,7 +4327,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="106305792"/>
+        <c:crossAx val="105077376"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4335,7 +4335,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="106305792"/>
+        <c:axId val="105077376"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4346,7 +4346,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="106304256"/>
+        <c:crossAx val="105075840"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4559,11 +4559,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="106349696"/>
-        <c:axId val="106351232"/>
+        <c:axId val="105104896"/>
+        <c:axId val="105106432"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="106349696"/>
+        <c:axId val="105104896"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4572,7 +4572,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="106351232"/>
+        <c:crossAx val="105106432"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4580,7 +4580,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="106351232"/>
+        <c:axId val="105106432"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4591,7 +4591,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="106349696"/>
+        <c:crossAx val="105104896"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -9446,7 +9446,7 @@
   </sheetPr>
   <dimension ref="A1:C624"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A238" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <sheetData>
@@ -41003,8 +41003,8 @@
   </sheetPr>
   <dimension ref="A1:G1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="D32" sqref="D32:D41"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -41012,6 +41012,7 @@
     <col min="2" max="2" width="16.28515625" customWidth="1"/>
     <col min="5" max="5" width="34.5703125" customWidth="1"/>
     <col min="6" max="6" width="29.28515625" customWidth="1"/>
+    <col min="7" max="7" width="12.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -41056,7 +41057,9 @@
       <c r="F2" t="s">
         <v>40</v>
       </c>
-      <c r="G2" s="22"/>
+      <c r="G2" s="22">
+        <v>35</v>
+      </c>
     </row>
     <row r="3" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A3" s="19" t="s">
@@ -41223,9 +41226,18 @@
       <c r="D11" s="20">
         <v>176456666.66666666</v>
       </c>
-      <c r="E11" s="22"/>
-      <c r="F11" s="22"/>
-      <c r="G11" s="22"/>
+      <c r="E11" s="26">
+        <f>E4/3*$G$2^3+E5/2*$G$2^2+E6*$G$2</f>
+        <v>3383333333.333334</v>
+      </c>
+      <c r="F11" s="26">
+        <f>F4/3*$G$2^3+F5/2*$G$2^2+F6*$G$2</f>
+        <v>3777254541.666666</v>
+      </c>
+      <c r="G11" s="26">
+        <f>(F11-E11)/E11</f>
+        <v>0.11642991379310305</v>
+      </c>
     </row>
     <row r="12" spans="1:7" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A12" s="21" t="s">
@@ -41790,6 +41802,12 @@
       <c r="D44" s="20">
         <v>88420013.333333328</v>
       </c>
+      <c r="E44" s="27">
+        <v>-2000000</v>
+      </c>
+      <c r="F44" s="27">
+        <v>-1000000</v>
+      </c>
     </row>
     <row r="45" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A45" s="21" t="s">
@@ -41804,6 +41822,12 @@
       <c r="D45" s="20">
         <v>106856800</v>
       </c>
+      <c r="E45" s="27">
+        <v>40000000</v>
+      </c>
+      <c r="F45" s="27">
+        <v>30000000</v>
+      </c>
     </row>
     <row r="46" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A46" s="21" t="s">
@@ -41818,6 +41842,12 @@
       <c r="D46" s="20">
         <v>122374058.66666667</v>
       </c>
+      <c r="E46" s="27">
+        <v>-9000000</v>
+      </c>
+      <c r="F46" s="27">
+        <v>-7000000</v>
+      </c>
     </row>
     <row r="47" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A47" s="21" t="s">
@@ -41942,6 +41972,12 @@
       <c r="D54" s="20">
         <v>68546801.333333328</v>
       </c>
+      <c r="E54" s="27">
+        <v>-2000000</v>
+      </c>
+      <c r="F54">
+        <v>-836107</v>
+      </c>
     </row>
     <row r="55" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A55" s="21" t="s">
@@ -41956,6 +41992,12 @@
       <c r="D55" s="20">
         <v>89735528</v>
       </c>
+      <c r="E55" s="27">
+        <v>30000000</v>
+      </c>
+      <c r="F55" s="27">
+        <v>30000000</v>
+      </c>
     </row>
     <row r="56" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A56" s="21" t="s">
@@ -41970,6 +42012,12 @@
       <c r="D56" s="20">
         <v>107951994.66666667</v>
       </c>
+      <c r="E56" s="27">
+        <v>-20000000</v>
+      </c>
+      <c r="F56" s="27">
+        <v>-10000000</v>
+      </c>
     </row>
     <row r="57" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A57" s="21" t="s">
@@ -42094,6 +42142,12 @@
       <c r="D64" s="20">
         <v>83319600</v>
       </c>
+      <c r="E64" s="27">
+        <v>-2000000</v>
+      </c>
+      <c r="F64" s="27">
+        <v>-1000000</v>
+      </c>
     </row>
     <row r="65" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A65" s="21" t="s">
@@ -42108,6 +42162,12 @@
       <c r="D65" s="20">
         <v>101628520</v>
       </c>
+      <c r="E65" s="27">
+        <v>30000000</v>
+      </c>
+      <c r="F65" s="27">
+        <v>30000000</v>
+      </c>
     </row>
     <row r="66" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A66" s="21" t="s">
@@ -42122,6 +42182,12 @@
       <c r="D66" s="20">
         <v>117678218.66666667</v>
       </c>
+      <c r="E66" s="27">
+        <v>-10000000</v>
+      </c>
+      <c r="F66" s="27">
+        <v>-8000000</v>
+      </c>
     </row>
     <row r="67" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A67" s="21" t="s">
@@ -42246,6 +42312,12 @@
       <c r="D74" s="20">
         <v>67506906.666666672</v>
       </c>
+      <c r="E74" s="27">
+        <v>-2000000</v>
+      </c>
+      <c r="F74">
+        <v>-979724</v>
+      </c>
     </row>
     <row r="75" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A75" s="21" t="s">
@@ -42260,6 +42332,12 @@
       <c r="D75" s="20">
         <v>90346386.666666672</v>
       </c>
+      <c r="E75" s="27">
+        <v>30000000</v>
+      </c>
+      <c r="F75" s="27">
+        <v>30000000</v>
+      </c>
     </row>
     <row r="76" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A76" s="21" t="s">
@@ -42274,6 +42352,12 @@
       <c r="D76" s="20">
         <v>108191776</v>
       </c>
+      <c r="E76" s="27">
+        <v>-20000000</v>
+      </c>
+      <c r="F76" s="27">
+        <v>-20000000</v>
+      </c>
     </row>
     <row r="77" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A77" s="21" t="s">
@@ -42398,6 +42482,12 @@
       <c r="D84" s="20">
         <v>48498204</v>
       </c>
+      <c r="E84">
+        <v>-948241</v>
+      </c>
+      <c r="F84">
+        <v>-428074</v>
+      </c>
     </row>
     <row r="85" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A85" s="21" t="s">
@@ -42412,6 +42502,12 @@
       <c r="D85" s="20">
         <v>68797344</v>
       </c>
+      <c r="E85" s="27">
+        <v>30000000</v>
+      </c>
+      <c r="F85" s="27">
+        <v>20000000</v>
+      </c>
     </row>
     <row r="86" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A86" s="21" t="s">
@@ -42426,6 +42522,12 @@
       <c r="D86" s="20">
         <v>88148970.666666672</v>
       </c>
+      <c r="E86" s="27">
+        <v>-20000000</v>
+      </c>
+      <c r="F86" s="27">
+        <v>-20000000</v>
+      </c>
     </row>
     <row r="87" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A87" s="21" t="s">
@@ -42550,6 +42652,12 @@
       <c r="D94" s="20">
         <v>82170426.666666672</v>
       </c>
+      <c r="E94" s="27">
+        <v>-2000000</v>
+      </c>
+      <c r="F94" s="27">
+        <v>-1000000</v>
+      </c>
     </row>
     <row r="95" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A95" s="19" t="s">
@@ -42564,6 +42672,12 @@
       <c r="D95" s="20">
         <v>104843181.33333333</v>
       </c>
+      <c r="E95" s="27">
+        <v>40000000</v>
+      </c>
+      <c r="F95" s="27">
+        <v>30000000</v>
+      </c>
     </row>
     <row r="96" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A96" s="19" t="s">
@@ -42578,6 +42692,12 @@
       <c r="D96" s="20">
         <v>122523629.33333333</v>
       </c>
+      <c r="E96" s="27">
+        <v>-20000000</v>
+      </c>
+      <c r="F96" s="27">
+        <v>-10000000</v>
+      </c>
     </row>
     <row r="97" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A97" s="19" t="s">
@@ -42702,6 +42822,12 @@
       <c r="D104" s="20">
         <v>68670088</v>
       </c>
+      <c r="E104" s="27">
+        <v>-1000000</v>
+      </c>
+      <c r="F104">
+        <v>-939908</v>
+      </c>
     </row>
     <row r="105" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A105" s="19" t="s">
@@ -42716,6 +42842,12 @@
       <c r="D105" s="20">
         <v>90714680</v>
       </c>
+      <c r="E105" s="27">
+        <v>30000000</v>
+      </c>
+      <c r="F105" s="27">
+        <v>30000000</v>
+      </c>
     </row>
     <row r="106" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A106" s="19" t="s">
@@ -42730,6 +42862,12 @@
       <c r="D106" s="20">
         <v>109522248</v>
       </c>
+      <c r="E106" s="27">
+        <v>-20000000</v>
+      </c>
+      <c r="F106" s="27">
+        <v>-20000000</v>
+      </c>
     </row>
     <row r="107" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A107" s="19" t="s">
@@ -42854,6 +42992,12 @@
       <c r="D114" s="20">
         <v>85882189.333333328</v>
       </c>
+      <c r="E114" s="27">
+        <v>-2000000</v>
+      </c>
+      <c r="F114">
+        <v>-967435</v>
+      </c>
     </row>
     <row r="115" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A115" s="23" t="s">
@@ -42868,6 +43012,12 @@
       <c r="D115" s="20">
         <v>110943453.33333333</v>
       </c>
+      <c r="E115" s="27">
+        <v>40000000</v>
+      </c>
+      <c r="F115" s="27">
+        <v>30000000</v>
+      </c>
     </row>
     <row r="116" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A116" s="23" t="s">
@@ -42882,6 +43032,12 @@
       <c r="D116" s="20">
         <v>132074026.66666667</v>
       </c>
+      <c r="E116" s="27">
+        <v>-20000000</v>
+      </c>
+      <c r="F116" s="27">
+        <v>-10000000</v>
+      </c>
     </row>
     <row r="117" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A117" s="23" t="s">
@@ -43006,6 +43162,12 @@
       <c r="D124" s="20">
         <v>51911365.333333336</v>
       </c>
+      <c r="E124" s="27">
+        <v>-1000000</v>
+      </c>
+      <c r="F124">
+        <v>-427586</v>
+      </c>
     </row>
     <row r="125" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A125" s="23" t="s">
@@ -43020,6 +43182,12 @@
       <c r="D125" s="20">
         <v>72927738.666666672</v>
       </c>
+      <c r="E125" s="27">
+        <v>30000000</v>
+      </c>
+      <c r="F125" s="27">
+        <v>20000000</v>
+      </c>
     </row>
     <row r="126" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A126" s="23" t="s">
@@ -43034,6 +43202,12 @@
       <c r="D126" s="20">
         <v>91642576</v>
       </c>
+      <c r="E126" s="27">
+        <v>-20000000</v>
+      </c>
+      <c r="F126" s="27">
+        <v>-10000000</v>
+      </c>
     </row>
     <row r="127" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A127" s="23" t="s">
@@ -43158,6 +43332,12 @@
       <c r="D134" s="20">
         <v>71516428</v>
       </c>
+      <c r="E134" s="27">
+        <v>-2000000</v>
+      </c>
+      <c r="F134">
+        <v>-811883</v>
+      </c>
     </row>
     <row r="135" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A135" s="23" t="s">
@@ -43172,6 +43352,12 @@
       <c r="D135" s="20">
         <v>96038792</v>
       </c>
+      <c r="E135" s="27">
+        <v>30000000</v>
+      </c>
+      <c r="F135" s="27">
+        <v>30000000</v>
+      </c>
     </row>
     <row r="136" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A136" s="23" t="s">
@@ -43186,6 +43372,12 @@
       <c r="D136" s="20">
         <v>117503653.33333333</v>
       </c>
+      <c r="E136" s="27">
+        <v>-20000000</v>
+      </c>
+      <c r="F136" s="27">
+        <v>-20000000</v>
+      </c>
     </row>
     <row r="137" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A137" s="23" t="s">
@@ -43310,8 +43502,14 @@
       <c r="D144" s="20">
         <v>74883325.333333328</v>
       </c>
-    </row>
-    <row r="145" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="E144" s="27">
+        <v>-2000000</v>
+      </c>
+      <c r="F144">
+        <v>-805942</v>
+      </c>
+    </row>
+    <row r="145" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A145" s="23" t="s">
         <v>36</v>
       </c>
@@ -43324,8 +43522,14 @@
       <c r="D145" s="20">
         <v>96577858.666666672</v>
       </c>
-    </row>
-    <row r="146" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="E145" s="27">
+        <v>30000000</v>
+      </c>
+      <c r="F145" s="27">
+        <v>30000000</v>
+      </c>
+    </row>
+    <row r="146" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A146" s="23" t="s">
         <v>36</v>
       </c>
@@ -43338,8 +43542,14 @@
       <c r="D146" s="20">
         <v>115449752</v>
       </c>
-    </row>
-    <row r="147" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="E146" s="27">
+        <v>-9000000</v>
+      </c>
+      <c r="F146" s="27">
+        <v>-10000000</v>
+      </c>
+    </row>
+    <row r="147" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A147" s="23" t="s">
         <v>36</v>
       </c>
@@ -43353,7 +43563,7 @@
         <v>132994093.33333333</v>
       </c>
     </row>
-    <row r="148" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="148" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A148" s="23" t="s">
         <v>36</v>
       </c>
@@ -43367,7 +43577,7 @@
         <v>150571136</v>
       </c>
     </row>
-    <row r="149" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="149" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A149" s="23" t="s">
         <v>36</v>
       </c>
@@ -43381,7 +43591,7 @@
         <v>167898874.66666666</v>
       </c>
     </row>
-    <row r="150" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="150" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A150" s="23" t="s">
         <v>36</v>
       </c>
@@ -43395,7 +43605,7 @@
         <v>185715877.33333334</v>
       </c>
     </row>
-    <row r="151" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="151" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A151" s="23" t="s">
         <v>36</v>
       </c>
@@ -43409,55 +43619,55 @@
         <v>205054170.66666666</v>
       </c>
     </row>
-    <row r="152" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="152" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A152" s="24"/>
       <c r="B152" s="24"/>
       <c r="C152" s="20"/>
       <c r="D152" s="20"/>
     </row>
-    <row r="153" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="153" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A153" s="24"/>
       <c r="B153" s="24"/>
       <c r="C153" s="20"/>
       <c r="D153" s="20"/>
     </row>
-    <row r="154" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="154" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A154" s="24"/>
       <c r="B154" s="24"/>
       <c r="C154" s="20"/>
       <c r="D154" s="20"/>
     </row>
-    <row r="155" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="155" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A155" s="24"/>
       <c r="B155" s="24"/>
       <c r="C155" s="20"/>
       <c r="D155" s="20"/>
     </row>
-    <row r="156" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="156" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A156" s="24"/>
       <c r="B156" s="24"/>
       <c r="C156" s="20"/>
       <c r="D156" s="20"/>
     </row>
-    <row r="157" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="157" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A157" s="24"/>
       <c r="B157" s="24"/>
       <c r="C157" s="20"/>
       <c r="D157" s="20"/>
     </row>
-    <row r="158" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="158" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A158" s="24"/>
       <c r="B158" s="24"/>
       <c r="C158" s="20"/>
       <c r="D158" s="20"/>
     </row>
-    <row r="159" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="159" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A159" s="24"/>
       <c r="B159" s="24"/>
       <c r="C159" s="20"/>
       <c r="D159" s="20"/>
     </row>
-    <row r="160" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="160" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A160" s="24"/>
       <c r="B160" s="24"/>
       <c r="C160" s="20"/>

</xml_diff>

<commit_message>
terminei dg 7.6 excel e sigma mas tem outliers errados
</commit_message>
<xml_diff>
--- a/doc/ACAP DG PH 7.6 31-03-21.xlsx
+++ b/doc/ACAP DG PH 7.6 31-03-21.xlsx
@@ -12,7 +12,6 @@
     <sheet name="Dados planilhados" sheetId="3" r:id="rId3"/>
     <sheet name="Feito com formula" sheetId="5" r:id="rId4"/>
     <sheet name="Dados sem e com ABAP" sheetId="4" r:id="rId5"/>
-    <sheet name="Plan1" sheetId="6" r:id="rId6"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'Dados planilhados'!$A$1:$H$1249</definedName>
@@ -28,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2878" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2890" uniqueCount="75">
   <si>
     <t>##BLOCKS= 1</t>
   </si>
@@ -218,6 +217,42 @@
   <si>
     <t xml:space="preserve"> 14144296.099 + (6109156.455 * 45) - (46988.421 * 45^2) </t>
   </si>
+  <si>
+    <t xml:space="preserve"> 10101261.300 + (4447317.269 * 45) - (41941.289 * 45^2) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">8688002.790 + (5573157.040 * 45) - (38037.042 * 45^2) </t>
+  </si>
+  <si>
+    <t>16348103.223 + (6212393.675 * 45) - (67690.648 * 45^2)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 16631358.078 + (6278005.618 * 45) - (37379.839 * 45^2) </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 2771017.964 + (4001238.845 * 45) - (35774.104 * 45^2) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">3764594.424 + (4494724.389 * 45) - (17544.174 * 45^2) </t>
+  </si>
+  <si>
+    <t>0.36 para 0.32</t>
+  </si>
+  <si>
+    <t xml:space="preserve">12013613.031 + (5702324.504 * 45) - (52914.994 * 45^2) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">6946080.229 + (5907759.378 * 45) - (33820.428 * 45^2) </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 18759245.822 + (4766241.431 * 45) - (48286.252 * 45^2) </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 6946080.229 + (5907759.378 * 45) - (33820.428 * 45^2) </t>
+  </si>
+  <si>
+    <t>0.25 PARA 0.23</t>
+  </si>
 </sst>
 </file>
 
@@ -225,7 +260,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="d\.m"/>
-    <numFmt numFmtId="169" formatCode="0.0000"/>
+    <numFmt numFmtId="165" formatCode="0.0000"/>
   </numFmts>
   <fonts count="13" x14ac:knownFonts="1">
     <font>
@@ -428,7 +463,7 @@
     <xf numFmtId="2" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="169" fontId="1" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="1" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="3" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
@@ -652,11 +687,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="94178304"/>
-        <c:axId val="94188288"/>
+        <c:axId val="100211712"/>
+        <c:axId val="100225792"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="94178304"/>
+        <c:axId val="100211712"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -665,7 +700,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="94188288"/>
+        <c:crossAx val="100225792"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -673,7 +708,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="94188288"/>
+        <c:axId val="100225792"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -684,7 +719,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="94178304"/>
+        <c:crossAx val="100211712"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -897,11 +932,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="103168256"/>
-        <c:axId val="103178240"/>
+        <c:axId val="102844672"/>
+        <c:axId val="102854656"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="103168256"/>
+        <c:axId val="102844672"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -910,7 +945,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="103178240"/>
+        <c:crossAx val="102854656"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -918,7 +953,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="103178240"/>
+        <c:axId val="102854656"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -929,7 +964,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="103168256"/>
+        <c:crossAx val="102844672"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1142,11 +1177,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="103209600"/>
-        <c:axId val="103092608"/>
+        <c:axId val="102877824"/>
+        <c:axId val="103416192"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="103209600"/>
+        <c:axId val="102877824"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1155,7 +1190,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="103092608"/>
+        <c:crossAx val="103416192"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1163,7 +1198,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="103092608"/>
+        <c:axId val="103416192"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1174,7 +1209,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="103209600"/>
+        <c:crossAx val="102877824"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1387,11 +1422,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="103107584"/>
-        <c:axId val="103113472"/>
+        <c:axId val="103431168"/>
+        <c:axId val="103441152"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="103107584"/>
+        <c:axId val="103431168"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1400,7 +1435,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="103113472"/>
+        <c:crossAx val="103441152"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1408,7 +1443,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="103113472"/>
+        <c:axId val="103441152"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1419,7 +1454,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="103107584"/>
+        <c:crossAx val="103431168"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1632,11 +1667,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="103144832"/>
-        <c:axId val="104465536"/>
+        <c:axId val="103488896"/>
+        <c:axId val="103494784"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="103144832"/>
+        <c:axId val="103488896"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1645,7 +1680,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="104465536"/>
+        <c:crossAx val="103494784"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1653,7 +1688,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="104465536"/>
+        <c:axId val="103494784"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1664,7 +1699,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="103144832"/>
+        <c:crossAx val="103488896"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1877,11 +1912,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="104513536"/>
-        <c:axId val="104515072"/>
+        <c:axId val="103538688"/>
+        <c:axId val="103540224"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="104513536"/>
+        <c:axId val="103538688"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1890,7 +1925,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="104515072"/>
+        <c:crossAx val="103540224"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1898,7 +1933,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="104515072"/>
+        <c:axId val="103540224"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1909,7 +1944,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="104513536"/>
+        <c:crossAx val="103538688"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2122,11 +2157,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="104558976"/>
-        <c:axId val="104560512"/>
+        <c:axId val="103584128"/>
+        <c:axId val="103585664"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="104558976"/>
+        <c:axId val="103584128"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2135,7 +2170,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="104560512"/>
+        <c:crossAx val="103585664"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2143,7 +2178,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="104560512"/>
+        <c:axId val="103585664"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2154,7 +2189,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="104558976"/>
+        <c:crossAx val="103584128"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2367,11 +2402,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="94207360"/>
-        <c:axId val="94221440"/>
+        <c:axId val="100253056"/>
+        <c:axId val="100304000"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="94207360"/>
+        <c:axId val="100253056"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2380,7 +2415,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="94221440"/>
+        <c:crossAx val="100304000"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2388,7 +2423,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="94221440"/>
+        <c:axId val="100304000"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2399,7 +2434,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="94207360"/>
+        <c:crossAx val="100253056"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2617,11 +2652,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="96051200"/>
-        <c:axId val="96052736"/>
+        <c:axId val="101646336"/>
+        <c:axId val="101647872"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="96051200"/>
+        <c:axId val="101646336"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2630,7 +2665,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="96052736"/>
+        <c:crossAx val="101647872"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2638,7 +2673,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="96052736"/>
+        <c:axId val="101647872"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2649,7 +2684,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="96051200"/>
+        <c:crossAx val="101646336"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2862,11 +2897,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="102066048"/>
-        <c:axId val="102067584"/>
+        <c:axId val="101687680"/>
+        <c:axId val="101689216"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="102066048"/>
+        <c:axId val="101687680"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2875,7 +2910,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="102067584"/>
+        <c:crossAx val="101689216"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2883,7 +2918,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="102067584"/>
+        <c:axId val="101689216"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2894,7 +2929,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="102066048"/>
+        <c:crossAx val="101687680"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3117,11 +3152,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="102582912"/>
-        <c:axId val="102584704"/>
+        <c:axId val="102381824"/>
+        <c:axId val="102387712"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="102582912"/>
+        <c:axId val="102381824"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3130,7 +3165,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="102584704"/>
+        <c:crossAx val="102387712"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3138,7 +3173,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="102584704"/>
+        <c:axId val="102387712"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3149,7 +3184,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="102582912"/>
+        <c:crossAx val="102381824"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3362,11 +3397,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="102624256"/>
-        <c:axId val="102961920"/>
+        <c:axId val="102419456"/>
+        <c:axId val="102429440"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="102624256"/>
+        <c:axId val="102419456"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3375,7 +3410,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="102961920"/>
+        <c:crossAx val="102429440"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3383,7 +3418,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="102961920"/>
+        <c:axId val="102429440"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3394,7 +3429,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="102624256"/>
+        <c:crossAx val="102419456"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3607,11 +3642,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="102988800"/>
-        <c:axId val="102998784"/>
+        <c:axId val="102464512"/>
+        <c:axId val="102486784"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="102988800"/>
+        <c:axId val="102464512"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3620,7 +3655,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="102998784"/>
+        <c:crossAx val="102486784"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3628,7 +3663,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="102998784"/>
+        <c:axId val="102486784"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3639,7 +3674,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="102988800"/>
+        <c:crossAx val="102464512"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3852,11 +3887,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="103020032"/>
-        <c:axId val="103021568"/>
+        <c:axId val="103624064"/>
+        <c:axId val="103629952"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="103020032"/>
+        <c:axId val="103624064"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3865,7 +3900,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="103021568"/>
+        <c:crossAx val="103629952"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3873,7 +3908,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="103021568"/>
+        <c:axId val="103629952"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3884,7 +3919,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="103020032"/>
+        <c:crossAx val="103624064"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4097,11 +4132,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="103061376"/>
-        <c:axId val="103062912"/>
+        <c:axId val="103669760"/>
+        <c:axId val="103671296"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="103061376"/>
+        <c:axId val="103669760"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4110,7 +4145,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="103062912"/>
+        <c:crossAx val="103671296"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4118,7 +4153,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="103062912"/>
+        <c:axId val="103671296"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4129,7 +4164,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="103061376"/>
+        <c:crossAx val="103669760"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -46463,8 +46498,8 @@
   </sheetPr>
   <dimension ref="A1:M1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C82" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="G101" sqref="G101"/>
+    <sheetView tabSelected="1" topLeftCell="D133" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="F154" sqref="F154"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -48813,6 +48848,12 @@
       <c r="D102" s="23">
         <v>5562600</v>
       </c>
+      <c r="E102" s="32" t="s">
+        <v>63</v>
+      </c>
+      <c r="F102" s="32" t="s">
+        <v>64</v>
+      </c>
       <c r="M102" s="23" t="b">
         <f t="shared" si="3"/>
         <v>0</v>
@@ -48849,6 +48890,12 @@
       <c r="D104" s="23">
         <v>64517574</v>
       </c>
+      <c r="E104" s="32">
+        <v>-41941289</v>
+      </c>
+      <c r="F104" s="32">
+        <v>-38037042</v>
+      </c>
       <c r="M104" s="23" t="b">
         <f t="shared" si="3"/>
         <v>0</v>
@@ -48867,6 +48914,12 @@
       <c r="D105" s="23">
         <v>86523307.666666672</v>
       </c>
+      <c r="E105" s="32">
+        <v>4447317269</v>
+      </c>
+      <c r="F105" s="32">
+        <v>5573157040</v>
+      </c>
       <c r="M105" s="23" t="b">
         <f t="shared" si="3"/>
         <v>0</v>
@@ -48885,6 +48938,12 @@
       <c r="D106" s="23">
         <v>105268716.33333333</v>
       </c>
+      <c r="E106" s="32">
+        <v>10101261300</v>
+      </c>
+      <c r="F106" s="32">
+        <v>8688002790</v>
+      </c>
       <c r="M106" s="23" t="b">
         <f t="shared" si="3"/>
         <v>0</v>
@@ -48959,15 +49018,15 @@
       </c>
       <c r="E110" s="32">
         <f>E104/3*$G$2^3+E105/2*$G$2^2+E106*$G$2</f>
-        <v>0</v>
+        <v>3683498839987.5</v>
       </c>
       <c r="F110" s="32">
         <f>F104/3*$G$2^3+F105/2*$G$2^2+F106*$G$2</f>
-        <v>0</v>
-      </c>
-      <c r="G110" s="24" t="e">
+        <v>4878406477800</v>
+      </c>
+      <c r="G110" s="24">
         <f>(F110-E110)/E110</f>
-        <v>#DIV/0!</v>
+        <v>0.32439473710179179</v>
       </c>
       <c r="M110" s="23" t="b">
         <f t="shared" si="3"/>
@@ -48987,9 +49046,18 @@
       <c r="D111" s="23">
         <v>185045421.66666666</v>
       </c>
-      <c r="E111" s="33"/>
-      <c r="F111" s="33"/>
-      <c r="G111" s="31"/>
+      <c r="E111" s="33">
+        <f xml:space="preserve"> 10101261.3*45 + (4447317.269/2 * 45^2) - (41941.289/3 * 45^3)</f>
+        <v>3683498839.9875002</v>
+      </c>
+      <c r="F111" s="33">
+        <f>8688002.79*45 + (5573157.04/2 * 45^2) - (38037.042/3 * 45^3)</f>
+        <v>4878406477.8000002</v>
+      </c>
+      <c r="G111" s="35">
+        <f>(F111-E111)/E111</f>
+        <v>0.32439473710179173</v>
+      </c>
       <c r="M111" s="23" t="b">
         <f t="shared" si="3"/>
         <v>0</v>
@@ -49008,6 +49076,12 @@
       <c r="D112" s="23">
         <v>8808033.833333334</v>
       </c>
+      <c r="E112" s="32" t="s">
+        <v>65</v>
+      </c>
+      <c r="F112" s="32" t="s">
+        <v>66</v>
+      </c>
       <c r="M112" s="23" t="b">
         <f t="shared" si="3"/>
         <v>0</v>
@@ -49044,6 +49118,12 @@
       <c r="D114" s="23">
         <v>81729675.333333328</v>
       </c>
+      <c r="E114" s="32">
+        <v>-67690648</v>
+      </c>
+      <c r="F114" s="32">
+        <v>-37379839</v>
+      </c>
       <c r="M114" s="23" t="b">
         <f t="shared" si="3"/>
         <v>0</v>
@@ -49062,6 +49142,12 @@
       <c r="D115" s="23">
         <v>106752081</v>
       </c>
+      <c r="E115" s="32">
+        <v>6212393675</v>
+      </c>
+      <c r="F115" s="32">
+        <v>6278005618</v>
+      </c>
       <c r="M115" s="23" t="b">
         <f t="shared" si="3"/>
         <v>0</v>
@@ -49080,6 +49166,12 @@
       <c r="D116" s="23">
         <v>127820495</v>
       </c>
+      <c r="E116" s="32">
+        <v>16348103223</v>
+      </c>
+      <c r="F116" s="32">
+        <v>16631358078</v>
+      </c>
       <c r="M116" s="23" t="b">
         <f t="shared" si="3"/>
         <v>0</v>
@@ -49154,15 +49246,15 @@
       </c>
       <c r="E120" s="32">
         <f>E114/3*$G$2^3+E115/2*$G$2^2+E116*$G$2</f>
-        <v>0</v>
+        <v>4969609807972.5</v>
       </c>
       <c r="F120" s="32">
         <f>F114/3*$G$2^3+F115/2*$G$2^2+F116*$G$2</f>
-        <v>0</v>
-      </c>
-      <c r="G120" s="24" t="e">
+        <v>5969479192110</v>
+      </c>
+      <c r="G120" s="24">
         <f>(F120-E120)/E120</f>
-        <v>#DIV/0!</v>
+        <v>0.20119675845243601</v>
       </c>
       <c r="M120" s="23" t="b">
         <f t="shared" si="3"/>
@@ -49182,9 +49274,18 @@
       <c r="D121" s="23">
         <v>228643949.66666666</v>
       </c>
-      <c r="E121" s="33"/>
-      <c r="F121" s="33"/>
-      <c r="G121" s="31"/>
+      <c r="E121" s="33">
+        <f>16348103.223*45 + (6212393.675/2 * 45^2) - (67690.648/3 * 45^3)</f>
+        <v>4969609807.9724998</v>
+      </c>
+      <c r="F121" s="33">
+        <f xml:space="preserve"> 16631358.078*45 + (6278005.618/2 * 45^2) - (37379.839/3 * 45^3)</f>
+        <v>5969479192.1099997</v>
+      </c>
+      <c r="G121" s="35">
+        <f>(F121-E121)/E121</f>
+        <v>0.20119675845243598</v>
+      </c>
       <c r="M121" s="23" t="b">
         <f t="shared" si="3"/>
         <v>0</v>
@@ -49203,6 +49304,12 @@
       <c r="D122" s="23">
         <v>3685920.6666666665</v>
       </c>
+      <c r="E122" s="32" t="s">
+        <v>67</v>
+      </c>
+      <c r="F122" s="32" t="s">
+        <v>68</v>
+      </c>
       <c r="M122" s="23" t="b">
         <f t="shared" si="3"/>
         <v>0</v>
@@ -49239,6 +49346,12 @@
       <c r="D124" s="23">
         <v>47758851.333333336</v>
       </c>
+      <c r="E124" s="32">
+        <v>-35774104</v>
+      </c>
+      <c r="F124" s="32">
+        <v>-17544174</v>
+      </c>
       <c r="M124" s="23" t="b">
         <f t="shared" si="3"/>
         <v>0</v>
@@ -49257,6 +49370,12 @@
       <c r="D125" s="23">
         <v>68736366.333333343</v>
       </c>
+      <c r="E125" s="32">
+        <v>4001238845</v>
+      </c>
+      <c r="F125" s="32">
+        <v>4494724389</v>
+      </c>
       <c r="M125" s="23" t="b">
         <f t="shared" si="3"/>
         <v>0</v>
@@ -49275,6 +49394,12 @@
       <c r="D126" s="23">
         <v>87389044.333333328</v>
       </c>
+      <c r="E126" s="32">
+        <v>2771017964</v>
+      </c>
+      <c r="F126" s="32">
+        <v>3764594424</v>
+      </c>
       <c r="M126" s="23" t="b">
         <f t="shared" si="3"/>
         <v>0</v>
@@ -49329,6 +49454,9 @@
       <c r="D129" s="23">
         <v>138039827</v>
       </c>
+      <c r="G129" s="36" t="s">
+        <v>69</v>
+      </c>
       <c r="M129" s="23" t="b">
         <f t="shared" si="3"/>
         <v>0</v>
@@ -49349,15 +49477,15 @@
       </c>
       <c r="E130" s="32">
         <f>E124/3*$G$2^3+E125/2*$G$2^2+E126*$G$2</f>
-        <v>0</v>
+        <v>3089311729942.5</v>
       </c>
       <c r="F130" s="32">
         <f>F124/3*$G$2^3+F125/2*$G$2^2+F126*$G$2</f>
-        <v>0</v>
-      </c>
-      <c r="G130" s="24" t="e">
+        <v>4187410907692.5</v>
+      </c>
+      <c r="G130" s="24">
         <f>(F130-E130)/E130</f>
-        <v>#DIV/0!</v>
+        <v>0.35545107575480522</v>
       </c>
       <c r="M130" s="23" t="b">
         <f t="shared" ref="M130:M151" si="4">IF(C130=D130,"igual")</f>
@@ -49377,9 +49505,18 @@
       <c r="D131" s="23">
         <v>171391821.66666666</v>
       </c>
-      <c r="E131" s="33"/>
-      <c r="F131" s="33"/>
-      <c r="G131" s="31"/>
+      <c r="E131" s="33">
+        <f xml:space="preserve"> 2771017.964*45 + (4001238.845/2 * 45^2) - (35774.104/3 * 45^3)</f>
+        <v>3089311729.9425001</v>
+      </c>
+      <c r="F131" s="33">
+        <f>3764594.424*45 + (4494724.389/2 * 45^2) - (17544.174/3 * 45^3)</f>
+        <v>4187410907.6925001</v>
+      </c>
+      <c r="G131" s="35">
+        <f>(F131-E131)/E131</f>
+        <v>0.35545107575480522</v>
+      </c>
       <c r="M131" s="23" t="b">
         <f t="shared" si="4"/>
         <v>0</v>
@@ -49398,6 +49535,12 @@
       <c r="D132" s="23">
         <v>5630426.833333334</v>
       </c>
+      <c r="E132" s="32" t="s">
+        <v>70</v>
+      </c>
+      <c r="F132" s="32" t="s">
+        <v>71</v>
+      </c>
       <c r="M132" s="23" t="b">
         <f t="shared" si="4"/>
         <v>0</v>
@@ -49434,6 +49577,12 @@
       <c r="D134" s="23">
         <v>63054108</v>
       </c>
+      <c r="E134" s="32">
+        <v>-52914994</v>
+      </c>
+      <c r="F134" s="32">
+        <v>-33820428</v>
+      </c>
       <c r="M134" s="23" t="b">
         <f t="shared" si="4"/>
         <v>0</v>
@@ -49452,6 +49601,12 @@
       <c r="D135" s="23">
         <v>91847419.666666672</v>
       </c>
+      <c r="E135" s="32">
+        <v>5702324504</v>
+      </c>
+      <c r="F135" s="32">
+        <v>5907759378</v>
+      </c>
       <c r="M135" s="23" t="b">
         <f t="shared" si="4"/>
         <v>0</v>
@@ -49470,6 +49625,12 @@
       <c r="D136" s="23">
         <v>113250121.66666666</v>
       </c>
+      <c r="E136" s="32">
+        <v>12013613031</v>
+      </c>
+      <c r="F136" s="32">
+        <v>6946080229</v>
+      </c>
       <c r="M136" s="23" t="b">
         <f t="shared" si="4"/>
         <v>0</v>
@@ -49544,15 +49705,15 @@
       </c>
       <c r="E140" s="32">
         <f>E134/3*$G$2^3+E135/2*$G$2^2+E136*$G$2</f>
-        <v>0</v>
+        <v>4706923203945</v>
       </c>
       <c r="F140" s="32">
         <f>F134/3*$G$2^3+F135/2*$G$2^2+F136*$G$2</f>
-        <v>0</v>
-      </c>
-      <c r="G140" s="24" t="e">
+        <v>5266884480030</v>
+      </c>
+      <c r="G140" s="24">
         <f>(F140-E140)/E140</f>
-        <v>#DIV/0!</v>
+        <v>0.11896545828826807</v>
       </c>
       <c r="M140" s="23" t="b">
         <f t="shared" si="4"/>
@@ -49572,9 +49733,18 @@
       <c r="D141" s="23">
         <v>206736307</v>
       </c>
-      <c r="E141" s="33"/>
-      <c r="F141" s="33"/>
-      <c r="G141" s="31"/>
+      <c r="E141" s="33">
+        <f>12013613.031*45 + (5702324.504/2 * 45^2) - (52914.994/3 * 45^3)</f>
+        <v>4706923203.9449997</v>
+      </c>
+      <c r="F141" s="33">
+        <f>6946080.229*45 + (5907759.378/2 * 45^2) - (33820.428/3 * 45^3)</f>
+        <v>5266884480.0299997</v>
+      </c>
+      <c r="G141" s="35">
+        <f>(F141-E141)/E141</f>
+        <v>0.11896545828826809</v>
+      </c>
       <c r="M141" s="23" t="b">
         <f t="shared" si="4"/>
         <v>0</v>
@@ -49593,6 +49763,12 @@
       <c r="D142" s="23">
         <v>7523110</v>
       </c>
+      <c r="E142" s="32" t="s">
+        <v>72</v>
+      </c>
+      <c r="F142" s="32" t="s">
+        <v>73</v>
+      </c>
       <c r="M142" s="23" t="b">
         <f t="shared" si="4"/>
         <v>0</v>
@@ -49629,6 +49805,12 @@
       <c r="D144" s="23">
         <v>70730811.333333328</v>
       </c>
+      <c r="E144" s="32">
+        <v>-48286252</v>
+      </c>
+      <c r="F144" s="32">
+        <v>-33820428</v>
+      </c>
       <c r="M144" s="23" t="b">
         <f t="shared" si="4"/>
         <v>0</v>
@@ -49647,6 +49829,12 @@
       <c r="D145" s="23">
         <v>92386486.333333343</v>
       </c>
+      <c r="E145" s="32">
+        <v>4766241431</v>
+      </c>
+      <c r="F145" s="32">
+        <v>5907759378</v>
+      </c>
       <c r="M145" s="23" t="b">
         <f t="shared" si="4"/>
         <v>0</v>
@@ -49665,6 +49853,12 @@
       <c r="D146" s="23">
         <v>111196220.33333333</v>
       </c>
+      <c r="E146" s="32">
+        <v>18759245822</v>
+      </c>
+      <c r="F146" s="32">
+        <v>6946080229</v>
+      </c>
       <c r="M146" s="23" t="b">
         <f t="shared" si="4"/>
         <v>0</v>
@@ -49719,6 +49913,9 @@
       <c r="D149" s="23">
         <v>163301779</v>
       </c>
+      <c r="G149" s="36" t="s">
+        <v>74</v>
+      </c>
       <c r="M149" s="23" t="b">
         <f t="shared" si="4"/>
         <v>0</v>
@@ -49739,15 +49936,15 @@
       </c>
       <c r="E150" s="32">
         <f>E144/3*$G$2^3+E145/2*$G$2^2+E146*$G$2</f>
-        <v>0</v>
+        <v>4203290606377.5</v>
       </c>
       <c r="F150" s="32">
         <f>F144/3*$G$2^3+F145/2*$G$2^2+F146*$G$2</f>
-        <v>0</v>
-      </c>
-      <c r="G150" s="24" t="e">
+        <v>5266884480030</v>
+      </c>
+      <c r="G150" s="24">
         <f>(F150-E150)/E150</f>
-        <v>#DIV/0!</v>
+        <v>0.25303838664848621</v>
       </c>
       <c r="M150" s="23" t="b">
         <f t="shared" si="4"/>
@@ -49767,9 +49964,18 @@
       <c r="D151" s="23">
         <v>200217165.66666666</v>
       </c>
-      <c r="E151" s="33"/>
-      <c r="F151" s="33"/>
-      <c r="G151" s="31"/>
+      <c r="E151" s="33">
+        <f xml:space="preserve"> 18759245.822*45 + (4766241.431/2 * 45^2) - (48286.252/3 * 45^3)</f>
+        <v>4203290606.3774996</v>
+      </c>
+      <c r="F151" s="33">
+        <f xml:space="preserve"> 6946080.229*45 + (5907759.378/2 * 45^2) - (33820.428/3 * 45^3)</f>
+        <v>5266884480.0299997</v>
+      </c>
+      <c r="G151" s="35">
+        <f>(F151-E151)/E151</f>
+        <v>0.25303838664848627</v>
+      </c>
       <c r="M151" s="23" t="b">
         <f t="shared" si="4"/>
         <v>0</v>
@@ -54874,21 +55080,4 @@
   <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
   <drawing r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K16" sqref="K16"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="2" width="12" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData/>
-  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
preparando para fazer as equacoes da 7.3
</commit_message>
<xml_diff>
--- a/doc/ACAP DG PH 7.6 31-03-21.xlsx
+++ b/doc/ACAP DG PH 7.6 31-03-21.xlsx
@@ -272,43 +272,51 @@
       <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="11"/>
       <color rgb="FFF48E3A"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="10"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="11"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
@@ -687,11 +695,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="100211712"/>
-        <c:axId val="100225792"/>
+        <c:axId val="31225344"/>
+        <c:axId val="31411200"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="100211712"/>
+        <c:axId val="31225344"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -700,7 +708,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="100225792"/>
+        <c:crossAx val="31411200"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -708,7 +716,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="100225792"/>
+        <c:axId val="31411200"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -719,7 +727,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="100211712"/>
+        <c:crossAx val="31225344"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -932,11 +940,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="102844672"/>
-        <c:axId val="102854656"/>
+        <c:axId val="30549120"/>
+        <c:axId val="30550656"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="102844672"/>
+        <c:axId val="30549120"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -945,7 +953,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="102854656"/>
+        <c:crossAx val="30550656"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -953,7 +961,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="102854656"/>
+        <c:axId val="30550656"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -964,7 +972,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="102844672"/>
+        <c:crossAx val="30549120"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1177,11 +1185,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="102877824"/>
-        <c:axId val="103416192"/>
+        <c:axId val="30602752"/>
+        <c:axId val="30604288"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="102877824"/>
+        <c:axId val="30602752"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1190,7 +1198,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="103416192"/>
+        <c:crossAx val="30604288"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1198,7 +1206,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="103416192"/>
+        <c:axId val="30604288"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1209,7 +1217,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="102877824"/>
+        <c:crossAx val="30602752"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1422,11 +1430,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="103431168"/>
-        <c:axId val="103441152"/>
+        <c:axId val="30644096"/>
+        <c:axId val="30645632"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="103431168"/>
+        <c:axId val="30644096"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1435,7 +1443,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="103441152"/>
+        <c:crossAx val="30645632"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1443,7 +1451,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="103441152"/>
+        <c:axId val="30645632"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1454,7 +1462,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="103431168"/>
+        <c:crossAx val="30644096"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1667,11 +1675,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="103488896"/>
-        <c:axId val="103494784"/>
+        <c:axId val="30673152"/>
+        <c:axId val="30674944"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="103488896"/>
+        <c:axId val="30673152"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1680,7 +1688,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="103494784"/>
+        <c:crossAx val="30674944"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1688,7 +1696,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="103494784"/>
+        <c:axId val="30674944"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1699,7 +1707,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="103488896"/>
+        <c:crossAx val="30673152"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1912,11 +1920,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="103538688"/>
-        <c:axId val="103540224"/>
+        <c:axId val="30710400"/>
+        <c:axId val="30716288"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="103538688"/>
+        <c:axId val="30710400"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1925,7 +1933,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="103540224"/>
+        <c:crossAx val="30716288"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1933,7 +1941,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="103540224"/>
+        <c:axId val="30716288"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1944,7 +1952,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="103538688"/>
+        <c:crossAx val="30710400"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2157,11 +2165,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="103584128"/>
-        <c:axId val="103585664"/>
+        <c:axId val="30743552"/>
+        <c:axId val="30786304"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="103584128"/>
+        <c:axId val="30743552"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2170,7 +2178,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="103585664"/>
+        <c:crossAx val="30786304"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2178,7 +2186,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="103585664"/>
+        <c:axId val="30786304"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2189,7 +2197,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="103584128"/>
+        <c:crossAx val="30743552"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2402,11 +2410,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="100253056"/>
-        <c:axId val="100304000"/>
+        <c:axId val="75191808"/>
+        <c:axId val="75193344"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="100253056"/>
+        <c:axId val="75191808"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2415,7 +2423,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="100304000"/>
+        <c:crossAx val="75193344"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2423,7 +2431,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="100304000"/>
+        <c:axId val="75193344"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2434,7 +2442,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="100253056"/>
+        <c:crossAx val="75191808"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2652,11 +2660,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="101646336"/>
-        <c:axId val="101647872"/>
+        <c:axId val="90145536"/>
+        <c:axId val="91474560"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="101646336"/>
+        <c:axId val="90145536"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2665,7 +2673,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="101647872"/>
+        <c:crossAx val="91474560"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2673,7 +2681,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="101647872"/>
+        <c:axId val="91474560"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2684,7 +2692,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="101646336"/>
+        <c:crossAx val="90145536"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2785,7 +2793,6 @@
             <c:dispRSqr val="1"/>
             <c:dispEq val="1"/>
             <c:trendlineLbl>
-              <c:layout/>
               <c:numFmt formatCode="General" sourceLinked="0"/>
             </c:trendlineLbl>
           </c:trendline>
@@ -2842,7 +2849,6 @@
             <c:dispRSqr val="1"/>
             <c:dispEq val="1"/>
             <c:trendlineLbl>
-              <c:layout/>
               <c:numFmt formatCode="General" sourceLinked="0"/>
             </c:trendlineLbl>
           </c:trendline>
@@ -2897,11 +2903,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="101687680"/>
-        <c:axId val="101689216"/>
+        <c:axId val="121584256"/>
+        <c:axId val="30327168"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="101687680"/>
+        <c:axId val="121584256"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2910,7 +2916,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="101689216"/>
+        <c:crossAx val="30327168"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2918,7 +2924,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="101689216"/>
+        <c:axId val="30327168"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2929,14 +2935,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="101687680"/>
+        <c:crossAx val="121584256"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -3040,7 +3045,6 @@
             <c:dispRSqr val="1"/>
             <c:dispEq val="1"/>
             <c:trendlineLbl>
-              <c:layout/>
               <c:numFmt formatCode="General" sourceLinked="0"/>
             </c:trendlineLbl>
           </c:trendline>
@@ -3097,7 +3101,6 @@
             <c:dispRSqr val="1"/>
             <c:dispEq val="1"/>
             <c:trendlineLbl>
-              <c:layout/>
               <c:numFmt formatCode="General" sourceLinked="0"/>
             </c:trendlineLbl>
           </c:trendline>
@@ -3152,11 +3155,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="102381824"/>
-        <c:axId val="102387712"/>
+        <c:axId val="30354816"/>
+        <c:axId val="30356608"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="102381824"/>
+        <c:axId val="30354816"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3165,7 +3168,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="102387712"/>
+        <c:crossAx val="30356608"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3173,7 +3176,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="102387712"/>
+        <c:axId val="30356608"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3184,14 +3187,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="102381824"/>
+        <c:crossAx val="30354816"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -3285,7 +3287,6 @@
             <c:dispRSqr val="1"/>
             <c:dispEq val="1"/>
             <c:trendlineLbl>
-              <c:layout/>
               <c:numFmt formatCode="General" sourceLinked="0"/>
             </c:trendlineLbl>
           </c:trendline>
@@ -3342,7 +3343,6 @@
             <c:dispRSqr val="1"/>
             <c:dispEq val="1"/>
             <c:trendlineLbl>
-              <c:layout/>
               <c:numFmt formatCode="General" sourceLinked="0"/>
             </c:trendlineLbl>
           </c:trendline>
@@ -3397,11 +3397,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="102419456"/>
-        <c:axId val="102429440"/>
+        <c:axId val="30429184"/>
+        <c:axId val="30430720"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="102419456"/>
+        <c:axId val="30429184"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3410,7 +3410,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="102429440"/>
+        <c:crossAx val="30430720"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3418,7 +3418,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="102429440"/>
+        <c:axId val="30430720"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3429,14 +3429,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="102419456"/>
+        <c:crossAx val="30429184"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -3642,11 +3641,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="102464512"/>
-        <c:axId val="102486784"/>
+        <c:axId val="30453760"/>
+        <c:axId val="30455296"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="102464512"/>
+        <c:axId val="30453760"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3655,7 +3654,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="102486784"/>
+        <c:crossAx val="30455296"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3663,7 +3662,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="102486784"/>
+        <c:axId val="30455296"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3674,7 +3673,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="102464512"/>
+        <c:crossAx val="30453760"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3887,11 +3886,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="103624064"/>
-        <c:axId val="103629952"/>
+        <c:axId val="30478720"/>
+        <c:axId val="30480256"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="103624064"/>
+        <c:axId val="30478720"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3900,7 +3899,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="103629952"/>
+        <c:crossAx val="30480256"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3908,7 +3907,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="103629952"/>
+        <c:axId val="30480256"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3919,7 +3918,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="103624064"/>
+        <c:crossAx val="30478720"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4132,11 +4131,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="103669760"/>
-        <c:axId val="103671296"/>
+        <c:axId val="30520064"/>
+        <c:axId val="30521600"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="103669760"/>
+        <c:axId val="30520064"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4145,7 +4144,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="103671296"/>
+        <c:crossAx val="30521600"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4153,7 +4152,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="103671296"/>
+        <c:axId val="30521600"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4164,7 +4163,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="103669760"/>
+        <c:crossAx val="30520064"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4844,8 +4843,8 @@
   </sheetPr>
   <dimension ref="A1:AE122"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView topLeftCell="A94" workbookViewId="0">
+      <selection activeCell="P19" sqref="P19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -14220,11 +14219,12 @@
   <dimension ref="A1:I2057"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="J11" sqref="J11"/>
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
+    <col min="3" max="3" width="20" customWidth="1"/>
     <col min="4" max="4" width="21.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -46498,8 +46498,8 @@
   </sheetPr>
   <dimension ref="A1:M1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D133" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="F154" sqref="F154"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
fazendo backup para passar para o meu computador
</commit_message>
<xml_diff>
--- a/doc/ACAP DG PH 7.6 31-03-21.xlsx
+++ b/doc/ACAP DG PH 7.6 31-03-21.xlsx
@@ -695,11 +695,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="31225344"/>
-        <c:axId val="31411200"/>
+        <c:axId val="31224576"/>
+        <c:axId val="31409280"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="31225344"/>
+        <c:axId val="31224576"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -708,7 +708,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="31411200"/>
+        <c:crossAx val="31409280"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -716,7 +716,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="31411200"/>
+        <c:axId val="31409280"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -727,7 +727,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="31225344"/>
+        <c:crossAx val="31224576"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -940,11 +940,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="30549120"/>
-        <c:axId val="30550656"/>
+        <c:axId val="30676480"/>
+        <c:axId val="30678016"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="30549120"/>
+        <c:axId val="30676480"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -953,7 +953,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="30550656"/>
+        <c:crossAx val="30678016"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -961,7 +961,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="30550656"/>
+        <c:axId val="30678016"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -972,7 +972,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="30549120"/>
+        <c:crossAx val="30676480"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1185,11 +1185,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="30602752"/>
-        <c:axId val="30604288"/>
+        <c:axId val="30726016"/>
+        <c:axId val="30727552"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="30602752"/>
+        <c:axId val="30726016"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1198,7 +1198,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="30604288"/>
+        <c:crossAx val="30727552"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1206,7 +1206,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="30604288"/>
+        <c:axId val="30727552"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1217,7 +1217,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="30602752"/>
+        <c:crossAx val="30726016"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1430,11 +1430,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="30644096"/>
-        <c:axId val="30645632"/>
+        <c:axId val="30800128"/>
+        <c:axId val="30826496"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="30644096"/>
+        <c:axId val="30800128"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1443,7 +1443,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="30645632"/>
+        <c:crossAx val="30826496"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1451,7 +1451,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="30645632"/>
+        <c:axId val="30826496"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1462,7 +1462,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="30644096"/>
+        <c:crossAx val="30800128"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1675,11 +1675,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="30673152"/>
-        <c:axId val="30674944"/>
+        <c:axId val="30853760"/>
+        <c:axId val="30855552"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="30673152"/>
+        <c:axId val="30853760"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1688,7 +1688,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="30674944"/>
+        <c:crossAx val="30855552"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1696,7 +1696,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="30674944"/>
+        <c:axId val="30855552"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1707,7 +1707,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="30673152"/>
+        <c:crossAx val="30853760"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1920,11 +1920,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="30710400"/>
-        <c:axId val="30716288"/>
+        <c:axId val="30870528"/>
+        <c:axId val="30929664"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="30710400"/>
+        <c:axId val="30870528"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1933,7 +1933,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="30716288"/>
+        <c:crossAx val="30929664"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1941,7 +1941,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="30716288"/>
+        <c:axId val="30929664"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1952,7 +1952,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="30710400"/>
+        <c:crossAx val="30870528"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2165,11 +2165,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="30743552"/>
-        <c:axId val="30786304"/>
+        <c:axId val="30940544"/>
+        <c:axId val="30954624"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="30743552"/>
+        <c:axId val="30940544"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2178,7 +2178,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="30786304"/>
+        <c:crossAx val="30954624"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2186,7 +2186,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="30786304"/>
+        <c:axId val="30954624"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2197,7 +2197,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="30743552"/>
+        <c:crossAx val="30940544"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2793,6 +2793,7 @@
             <c:dispRSqr val="1"/>
             <c:dispEq val="1"/>
             <c:trendlineLbl>
+              <c:layout/>
               <c:numFmt formatCode="General" sourceLinked="0"/>
             </c:trendlineLbl>
           </c:trendline>
@@ -2849,6 +2850,7 @@
             <c:dispRSqr val="1"/>
             <c:dispEq val="1"/>
             <c:trendlineLbl>
+              <c:layout/>
               <c:numFmt formatCode="General" sourceLinked="0"/>
             </c:trendlineLbl>
           </c:trendline>
@@ -2904,7 +2906,7 @@
         <c:marker val="1"/>
         <c:smooth val="0"/>
         <c:axId val="121584256"/>
-        <c:axId val="30327168"/>
+        <c:axId val="163320192"/>
       </c:lineChart>
       <c:catAx>
         <c:axId val="121584256"/>
@@ -2916,7 +2918,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="30327168"/>
+        <c:crossAx val="163320192"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2924,7 +2926,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="30327168"/>
+        <c:axId val="163320192"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2942,6 +2944,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -3045,6 +3048,7 @@
             <c:dispRSqr val="1"/>
             <c:dispEq val="1"/>
             <c:trendlineLbl>
+              <c:layout/>
               <c:numFmt formatCode="General" sourceLinked="0"/>
             </c:trendlineLbl>
           </c:trendline>
@@ -3101,6 +3105,7 @@
             <c:dispRSqr val="1"/>
             <c:dispEq val="1"/>
             <c:trendlineLbl>
+              <c:layout/>
               <c:numFmt formatCode="General" sourceLinked="0"/>
             </c:trendlineLbl>
           </c:trendline>
@@ -3155,11 +3160,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="30354816"/>
-        <c:axId val="30356608"/>
+        <c:axId val="30522752"/>
+        <c:axId val="30524544"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="30354816"/>
+        <c:axId val="30522752"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3168,7 +3173,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="30356608"/>
+        <c:crossAx val="30524544"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3176,7 +3181,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="30356608"/>
+        <c:axId val="30524544"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3187,13 +3192,14 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="30354816"/>
+        <c:crossAx val="30522752"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -3287,6 +3293,7 @@
             <c:dispRSqr val="1"/>
             <c:dispEq val="1"/>
             <c:trendlineLbl>
+              <c:layout/>
               <c:numFmt formatCode="General" sourceLinked="0"/>
             </c:trendlineLbl>
           </c:trendline>
@@ -3343,6 +3350,7 @@
             <c:dispRSqr val="1"/>
             <c:dispEq val="1"/>
             <c:trendlineLbl>
+              <c:layout/>
               <c:numFmt formatCode="General" sourceLinked="0"/>
             </c:trendlineLbl>
           </c:trendline>
@@ -3397,11 +3405,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="30429184"/>
-        <c:axId val="30430720"/>
+        <c:axId val="30548352"/>
+        <c:axId val="30549888"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="30429184"/>
+        <c:axId val="30548352"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3410,7 +3418,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="30430720"/>
+        <c:crossAx val="30549888"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3418,7 +3426,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="30430720"/>
+        <c:axId val="30549888"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3429,13 +3437,14 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="30429184"/>
+        <c:crossAx val="30548352"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -3641,11 +3650,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="30453760"/>
-        <c:axId val="30455296"/>
+        <c:axId val="30589696"/>
+        <c:axId val="30591232"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="30453760"/>
+        <c:axId val="30589696"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3654,7 +3663,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="30455296"/>
+        <c:crossAx val="30591232"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3662,7 +3671,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="30455296"/>
+        <c:axId val="30591232"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3673,7 +3682,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="30453760"/>
+        <c:crossAx val="30589696"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3886,11 +3895,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="30478720"/>
-        <c:axId val="30480256"/>
+        <c:axId val="30618368"/>
+        <c:axId val="30619904"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="30478720"/>
+        <c:axId val="30618368"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3899,7 +3908,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="30480256"/>
+        <c:crossAx val="30619904"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3907,7 +3916,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="30480256"/>
+        <c:axId val="30619904"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3918,7 +3927,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="30478720"/>
+        <c:crossAx val="30618368"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4131,11 +4140,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="30520064"/>
-        <c:axId val="30521600"/>
+        <c:axId val="30655616"/>
+        <c:axId val="30657152"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="30520064"/>
+        <c:axId val="30655616"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4144,7 +4153,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="30521600"/>
+        <c:crossAx val="30657152"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4152,7 +4161,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="30521600"/>
+        <c:axId val="30657152"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4163,7 +4172,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="30520064"/>
+        <c:crossAx val="30655616"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -46498,8 +46507,8 @@
   </sheetPr>
   <dimension ref="A1:M1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+    <sheetView tabSelected="1" topLeftCell="B37" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2:D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>